<commit_message>
Updated concurets analysis sheet
Added page "Таблиця"
</commit_message>
<xml_diff>
--- a/Documets/Concurents pros&cons.xlsx
+++ b/Documets/Concurents pros&cons.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
+    <sheet name="Загально" sheetId="1" r:id="rId1"/>
+    <sheet name="Таблиця" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>Плюси</t>
   </si>
@@ -144,6 +145,48 @@
   </si>
   <si>
     <t>не реалізує.</t>
+  </si>
+  <si>
+    <t>Можливість &gt;</t>
+  </si>
+  <si>
+    <t>Назва програми v</t>
+  </si>
+  <si>
+    <t>Зміст</t>
+  </si>
+  <si>
+    <t>Закладка</t>
+  </si>
+  <si>
+    <t>Теми</t>
+  </si>
+  <si>
+    <t>Зміна шрифта</t>
+  </si>
+  <si>
+    <t>Багатоформатність</t>
+  </si>
+  <si>
+    <t>Фільтрування</t>
+  </si>
+  <si>
+    <t>Виділення тексту кольором</t>
+  </si>
+  <si>
+    <t>Виділення і переклад тексту</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Онлайн</t>
+  </si>
+  <si>
+    <t>+ (за джерелом)</t>
   </si>
 </sst>
 </file>
@@ -186,7 +229,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -212,11 +255,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
@@ -230,6 +293,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -512,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,4 +771,182 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>